<commit_message>
Make WithCustomValueBinder possible on exports as well
</commit_message>
<xml_diff>
--- a/tests/Data/Disks/Local/value-binder-import.xlsx
+++ b/tests/Data/Disks/Local/value-binder-import.xlsx
@@ -31,10 +31,25 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -55,14 +70,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -360,10 +381,13 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -382,16 +406,17 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>3</v>
+      <c r="A3" s="2">
+        <v>43318.772060185183</v>
+      </c>
+      <c r="B3" s="3">
+        <v>43319</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>